<commit_message>
Added extended use case for profile
</commit_message>
<xml_diff>
--- a/Docs/Extended Use Case.xlsx
+++ b/Docs/Extended Use Case.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>UC : Submit bug / change report</t>
   </si>
@@ -55,6 +55,33 @@
   </si>
   <si>
     <t>7.  TUCEW the user reading the confirmation message.</t>
+  </si>
+  <si>
+    <t>UC : View profile and statistics</t>
+  </si>
+  <si>
+    <t>0.  System displays the main screen.</t>
+  </si>
+  <si>
+    <t>1.  TUCBW the user clicking on the profile button</t>
+  </si>
+  <si>
+    <t>2. The user's profile is displayed with basic information.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.  The user clicks the statistics button </t>
+  </si>
+  <si>
+    <t>4.  Total statistics such as total chip count and total wins/losses are displayed, along with a list of games.</t>
+  </si>
+  <si>
+    <t>5.  The user clicks on one of the individual games.</t>
+  </si>
+  <si>
+    <t>6.  Detailed statistics for that game are displayed, such as chips won or lost, wins and losses, and sessions played.</t>
+  </si>
+  <si>
+    <t>7.  TUCEW the user reading the statistics and exploring further to additional game types</t>
   </si>
 </sst>
 </file>
@@ -535,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C8"/>
+  <dimension ref="B1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,9 +624,61 @@
       </c>
       <c r="C8" s="6"/>
     </row>
+    <row r="9" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="10"/>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="1"/>
+      <c r="C12" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B10:C10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Changes to Euchre and Use Case Documents
</commit_message>
<xml_diff>
--- a/Docs/Extended Use Case.xlsx
+++ b/Docs/Extended Use Case.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
   <si>
     <t>UC : Submit bug / change report</t>
   </si>
@@ -63,15 +63,9 @@
     <t>0.  System displays the main screen.</t>
   </si>
   <si>
-    <t>1.  TUCBW the user clicking on the profile button</t>
-  </si>
-  <si>
     <t>2. The user's profile is displayed with basic information.</t>
   </si>
   <si>
-    <t xml:space="preserve">3.  The user clicks the statistics button </t>
-  </si>
-  <si>
     <t>4.  Total statistics such as total chip count and total wins/losses are displayed, along with a list of games.</t>
   </si>
   <si>
@@ -81,7 +75,100 @@
     <t>6.  Detailed statistics for that game are displayed, such as chips won or lost, wins and losses, and sessions played.</t>
   </si>
   <si>
-    <t>7.  TUCEW the user reading the statistics and exploring further to additional game types</t>
+    <t>UC: Change Account Settings</t>
+  </si>
+  <si>
+    <t>Actor: User</t>
+  </si>
+  <si>
+    <t>System: Card Game System</t>
+  </si>
+  <si>
+    <t>1.  TUCBW the user clicking on Change Account Settings button.</t>
+  </si>
+  <si>
+    <t>2.  User is taken to Account Settings Page with the following options:
+    2a.  Change account password.
+    2b.  Change account name.
+    2c.  Change security questions.
+    2d.  Change account email.</t>
+  </si>
+  <si>
+    <t>3.  User selects one of the following options:
+    3a.  Change account password.
+    3b.  Change account name.
+    3c.  Change security questions.
+    3d.  Change account email.</t>
+  </si>
+  <si>
+    <t>4.  System displays form depending on user's choice:
+    4a.  Change account password form.
+    4b.  Change account name form.
+    4c.  Change security questions form.
+    4d.  Change account email form.</t>
+  </si>
+  <si>
+    <t>5.  User fills out form and submits it.</t>
+  </si>
+  <si>
+    <t>6.  System displays confirmation message.</t>
+  </si>
+  <si>
+    <t>1.  TUCBW the user clicking on the profile button.</t>
+  </si>
+  <si>
+    <t>3.  The user clicks the statistics button.</t>
+  </si>
+  <si>
+    <t>7.  TUCEW the user reading the statistics and exploring further to additional game types.</t>
+  </si>
+  <si>
+    <t>0.  System displays Profile page.</t>
+  </si>
+  <si>
+    <t>UC:  Join a Table</t>
+  </si>
+  <si>
+    <t>3.  The user chooses a game they would like to play.</t>
+  </si>
+  <si>
+    <t>7.  The user begins to play the game.</t>
+  </si>
+  <si>
+    <t>UC:  Message Other Users</t>
+  </si>
+  <si>
+    <t>Actor:  User</t>
+  </si>
+  <si>
+    <t>1.  TUCBW the user clicking Start Playing Now</t>
+  </si>
+  <si>
+    <t>5.  The user clicks Join Table on the table they would like to play at.</t>
+  </si>
+  <si>
+    <t>0.  System displays a game/table.</t>
+  </si>
+  <si>
+    <t>3.  The user reads the messages sent by other users.</t>
+  </si>
+  <si>
+    <t>0.  System displays the home screen. (Figure 1)</t>
+  </si>
+  <si>
+    <t>2.  The system displays the page with a list of available games. (Figure 2)</t>
+  </si>
+  <si>
+    <t>4.  The system displays a list of tables based on the chosen game. (Figure 3)</t>
+  </si>
+  <si>
+    <t>6.  The system displays the game and the table to the user. (Figure 4)</t>
+  </si>
+  <si>
+    <t>1.  The user clicks on the chat text input field, types a message, and clicks send. (Figure 5)</t>
+  </si>
+  <si>
+    <t>2.  The system displays the message entered to everyone at the table. (Figure 4)</t>
   </si>
 </sst>
 </file>
@@ -105,7 +192,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -229,11 +316,67 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -246,12 +389,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -260,6 +397,54 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -562,10 +747,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C16"/>
+  <dimension ref="B1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,24 +758,24 @@
     <col min="2" max="3" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="1" spans="2:3" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="10"/>
+      <c r="C2" s="8"/>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
-      <c r="C4" s="2" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -603,85 +788,238 @@
       </c>
     </row>
     <row r="6" spans="2:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="6"/>
+      <c r="C8" s="14"/>
     </row>
     <row r="9" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="10"/>
+      <c r="C10" s="8"/>
     </row>
     <row r="11" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="16" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
-      <c r="C12" s="2" t="s">
+      <c r="B12" s="3"/>
+      <c r="C12" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="4" t="s">
+    </row>
+    <row r="14" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B14" s="1" t="s">
+    <row r="15" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C15" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="2:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="B15" s="1" t="s">
+    <row r="16" spans="2:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="14"/>
+    </row>
+    <row r="17" spans="2:3" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+    </row>
+    <row r="18" spans="2:3" ht="44.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C19" s="10"/>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="11" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="16" spans="2:3" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="5" t="s">
+      <c r="C20" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="6"/>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="1"/>
+      <c r="C21" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="B22" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" s="14"/>
+    </row>
+    <row r="26" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="21"/>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B29" s="3"/>
+      <c r="C29" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B30" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B31" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="B32" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33" s="14"/>
+    </row>
+    <row r="34" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="18"/>
+      <c r="C34" s="18"/>
+    </row>
+    <row r="35" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" s="21"/>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" s="23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="3"/>
+      <c r="C37" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B38" s="17" t="s">
+        <v>43</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B35:C35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;RRyan Bickham
+Nicholas Borushko
+Ryan Gillett
+Andrew Haeger</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 

</xml_diff>